<commit_message>
--Bugfix related to MSATollTravelDisutilityCalculator, updated to work with libraries of 0.9.0-SNAPSHOT version of MATSim.
--Discovered bug in the floor field diffusion: it provides problems in
case of adjoined intermediate targets. Environment files of Braess and
Daganzo experiments have been updated as a workaround, but the problem
persists for the time being.

--Last updates to the files related to the Staten Island scenario
</commit_message>
<xml_diff>
--- a/src/main/resources/visualizer.xlsx
+++ b/src/main/resources/visualizer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\git\matsim-org\matsim\playgrounds\lcrociani\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\git\CACrowd\casim\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">environmentGrid!$A$1:$IR$103</definedName>
-    <definedName name="ABMUS_PG_station_separated" localSheetId="0">environmentGrid!$A$1:$IR$103</definedName>
+    <definedName name="ABMUS_PG_station_largeStairs" localSheetId="0">environmentGrid!$A$1:$OS$103</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -24,9 +24,166 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="ABMUS_PG_station_separated" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="C:\Users\Luca\git\matsim-org\matsim\playgrounds\lcrociani\src\main\resources\ABMUS_PG_station_separated.csv" thousands="'" semicolon="1">
-      <textFields count="252">
+  <connection id="1" name="ABMUS_PG_station_largeStairs" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\Luca\git\CACrowd\casim\src\main\resources\ABMUS_PG_station_largeStairs.csv" thousands="'" semicolon="1">
+      <textFields count="409">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -813,25 +970,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -919,7 +1062,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABMUS_PG_station_separated" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ABMUS_PG_station_largeStairs" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1211,13 +1354,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:OS103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="252" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="252" width="2.26171875" bestFit="1" customWidth="1"/>
     <col min="253" max="253" width="3" customWidth="1"/>
     <col min="254" max="270" width="3" bestFit="1" customWidth="1"/>
     <col min="271" max="420" width="2.26171875" bestFit="1" customWidth="1"/>
@@ -1276,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="R1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S1">
         <v>-1</v>
@@ -2034,10 +2175,10 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S2">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -2049,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="W2">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X2">
         <v>0</v>
@@ -2792,10 +2933,10 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S3">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -2807,7 +2948,7 @@
         <v>0</v>
       </c>
       <c r="W3">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X3">
         <v>0</v>
@@ -3550,10 +3691,10 @@
         <v>0</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S4">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -3565,7 +3706,7 @@
         <v>0</v>
       </c>
       <c r="W4">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -4308,10 +4449,10 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S5">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -4323,7 +4464,7 @@
         <v>0</v>
       </c>
       <c r="W5">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X5">
         <v>0</v>
@@ -5066,10 +5207,10 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S6">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -5081,7 +5222,7 @@
         <v>0</v>
       </c>
       <c r="W6">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -5824,10 +5965,10 @@
         <v>0</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S7">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -5839,7 +5980,7 @@
         <v>0</v>
       </c>
       <c r="W7">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X7">
         <v>0</v>
@@ -6582,10 +6723,10 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S8">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -6597,7 +6738,7 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X8">
         <v>0</v>
@@ -7340,10 +7481,10 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S9">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T9">
         <v>0</v>
@@ -7355,7 +7496,7 @@
         <v>0</v>
       </c>
       <c r="W9">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X9">
         <v>0</v>
@@ -8099,10 +8240,10 @@
         <v>0</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S10">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -8114,7 +8255,7 @@
         <v>0</v>
       </c>
       <c r="W10">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X10">
         <v>0</v>
@@ -8857,10 +8998,10 @@
         <v>0</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S11">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T11">
         <v>0</v>
@@ -8872,7 +9013,7 @@
         <v>0</v>
       </c>
       <c r="W11">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X11">
         <v>0</v>
@@ -9615,10 +9756,10 @@
         <v>0</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S12">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T12">
         <v>0</v>
@@ -9630,7 +9771,7 @@
         <v>0</v>
       </c>
       <c r="W12">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X12">
         <v>0</v>
@@ -10373,10 +10514,10 @@
         <v>0</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S13">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T13">
         <v>0</v>
@@ -10388,7 +10529,7 @@
         <v>0</v>
       </c>
       <c r="W13">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X13">
         <v>0</v>
@@ -11131,31 +11272,31 @@
         <v>0</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S14">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="U14">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="V14">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="W14">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X14">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="Y14">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="Z14">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="AA14">
         <v>-1</v>
@@ -11889,10 +12030,10 @@
         <v>0</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S15">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T15">
         <v>0</v>
@@ -11904,7 +12045,7 @@
         <v>0</v>
       </c>
       <c r="W15">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X15">
         <v>0</v>
@@ -12647,10 +12788,10 @@
         <v>0</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S16">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T16">
         <v>0</v>
@@ -12662,7 +12803,7 @@
         <v>0</v>
       </c>
       <c r="W16">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X16">
         <v>0</v>
@@ -13405,10 +13546,10 @@
         <v>0</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S17">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T17">
         <v>0</v>
@@ -13420,7 +13561,7 @@
         <v>0</v>
       </c>
       <c r="W17">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X17">
         <v>0</v>
@@ -14163,10 +14304,10 @@
         <v>0</v>
       </c>
       <c r="R18">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S18">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T18">
         <v>0</v>
@@ -14178,7 +14319,7 @@
         <v>0</v>
       </c>
       <c r="W18">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X18">
         <v>0</v>
@@ -14921,10 +15062,10 @@
         <v>0</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S19">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T19">
         <v>0</v>
@@ -14936,7 +15077,7 @@
         <v>0</v>
       </c>
       <c r="W19">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X19">
         <v>0</v>
@@ -15679,10 +15820,10 @@
         <v>0</v>
       </c>
       <c r="R20">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="S20">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="T20">
         <v>0</v>
@@ -15694,7 +15835,7 @@
         <v>0</v>
       </c>
       <c r="W20">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="X20">
         <v>0</v>
@@ -16440,7 +16581,7 @@
         <v>-1</v>
       </c>
       <c r="S21">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="T21">
         <v>-4</v>
@@ -16452,7 +16593,7 @@
         <v>-4</v>
       </c>
       <c r="W21">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="X21">
         <v>-4</v>
@@ -17198,7 +17339,7 @@
         <v>-1</v>
       </c>
       <c r="S22">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T22">
         <v>0</v>
@@ -17956,7 +18097,7 @@
         <v>-1</v>
       </c>
       <c r="S23">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T23">
         <v>0</v>
@@ -18714,7 +18855,7 @@
         <v>-1</v>
       </c>
       <c r="S24">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T24">
         <v>0</v>
@@ -19472,7 +19613,7 @@
         <v>-1</v>
       </c>
       <c r="S25">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T25">
         <v>0</v>
@@ -20230,7 +20371,7 @@
         <v>-1</v>
       </c>
       <c r="S26">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T26">
         <v>0</v>
@@ -20988,7 +21129,7 @@
         <v>-1</v>
       </c>
       <c r="S27">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T27">
         <v>0</v>
@@ -21746,7 +21887,7 @@
         <v>-1</v>
       </c>
       <c r="S28">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T28">
         <v>0</v>
@@ -22504,7 +22645,7 @@
         <v>-1</v>
       </c>
       <c r="S29">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T29">
         <v>0</v>
@@ -23262,7 +23403,7 @@
         <v>-1</v>
       </c>
       <c r="S30">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T30">
         <v>0</v>
@@ -24020,7 +24161,7 @@
         <v>-1</v>
       </c>
       <c r="S31">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T31">
         <v>0</v>
@@ -24778,7 +24919,7 @@
         <v>-1</v>
       </c>
       <c r="S32">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T32">
         <v>0</v>
@@ -25536,7 +25677,7 @@
         <v>-1</v>
       </c>
       <c r="S33">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T33">
         <v>0</v>
@@ -26294,7 +26435,7 @@
         <v>-1</v>
       </c>
       <c r="S34">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T34">
         <v>0</v>
@@ -27052,7 +27193,7 @@
         <v>-1</v>
       </c>
       <c r="S35">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T35">
         <v>0</v>
@@ -27810,7 +27951,7 @@
         <v>-1</v>
       </c>
       <c r="S36">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T36">
         <v>0</v>
@@ -28568,7 +28709,7 @@
         <v>-1</v>
       </c>
       <c r="S37">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T37">
         <v>0</v>
@@ -29326,7 +29467,7 @@
         <v>-1</v>
       </c>
       <c r="S38">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T38">
         <v>0</v>
@@ -30084,7 +30225,7 @@
         <v>-1</v>
       </c>
       <c r="S39">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T39">
         <v>0</v>
@@ -30842,7 +30983,7 @@
         <v>-1</v>
       </c>
       <c r="S40">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T40">
         <v>0</v>
@@ -31600,7 +31741,7 @@
         <v>-1</v>
       </c>
       <c r="S41">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T41">
         <v>0</v>
@@ -32358,7 +32499,7 @@
         <v>-1</v>
       </c>
       <c r="S42">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T42">
         <v>0</v>
@@ -33116,7 +33257,7 @@
         <v>-1</v>
       </c>
       <c r="S43">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T43">
         <v>0</v>
@@ -33874,7 +34015,7 @@
         <v>-1</v>
       </c>
       <c r="S44">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T44">
         <v>0</v>
@@ -34632,7 +34773,7 @@
         <v>-1</v>
       </c>
       <c r="S45">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T45">
         <v>0</v>
@@ -35390,7 +35531,7 @@
         <v>-1</v>
       </c>
       <c r="S46">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T46">
         <v>0</v>
@@ -36148,7 +36289,7 @@
         <v>-1</v>
       </c>
       <c r="S47">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T47">
         <v>0</v>
@@ -36906,7 +37047,7 @@
         <v>-1</v>
       </c>
       <c r="S48">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T48">
         <v>0</v>
@@ -37664,7 +37805,7 @@
         <v>-1</v>
       </c>
       <c r="S49">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T49">
         <v>0</v>
@@ -38422,7 +38563,7 @@
         <v>-1</v>
       </c>
       <c r="S50">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="T50">
         <v>0</v>
@@ -39180,7 +39321,7 @@
         <v>-1</v>
       </c>
       <c r="S51">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="T51">
         <v>-4</v>
@@ -39192,7 +39333,7 @@
         <v>-4</v>
       </c>
       <c r="W51">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="X51">
         <v>-4</v>
@@ -39950,7 +40091,7 @@
         <v>0</v>
       </c>
       <c r="W52">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X52">
         <v>0</v>
@@ -40708,7 +40849,7 @@
         <v>0</v>
       </c>
       <c r="W53">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X53">
         <v>0</v>
@@ -41466,7 +41607,7 @@
         <v>0</v>
       </c>
       <c r="W54">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X54">
         <v>0</v>
@@ -42224,280 +42365,280 @@
         <v>0</v>
       </c>
       <c r="W55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Y55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA55">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AB55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AE55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AF55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AG55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AH55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AI55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AK55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AL55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AM55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AN55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AO55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AP55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AQ55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AS55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AT55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AU55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AV55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AW55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AX55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AY55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AZ55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BA55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BB55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BC55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BD55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BE55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BF55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BG55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BH55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BI55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BJ55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BK55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BL55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BM55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BN55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BO55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BP55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BQ55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BR55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BS55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BT55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BU55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BV55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BW55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BX55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BY55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BZ55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CA55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CB55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CC55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CD55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CE55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CF55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CG55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CH55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CI55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CJ55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CK55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CL55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CM55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CN55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CO55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CP55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CQ55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CR55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CS55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CT55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CU55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CV55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CW55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CX55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CY55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="CZ55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DA55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DB55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DC55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DD55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DE55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DF55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DG55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DH55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DI55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DJ55">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="DK55">
         <v>-1</v>
@@ -42587,40 +42728,40 @@
         <v>-1</v>
       </c>
       <c r="EN55">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="EO55">
+        <v>0</v>
+      </c>
+      <c r="EP55">
+        <v>0</v>
+      </c>
+      <c r="EQ55">
+        <v>0</v>
+      </c>
+      <c r="ER55">
+        <v>0</v>
+      </c>
+      <c r="ES55">
+        <v>0</v>
+      </c>
+      <c r="ET55">
+        <v>0</v>
+      </c>
+      <c r="EU55">
+        <v>0</v>
+      </c>
+      <c r="EV55">
+        <v>0</v>
+      </c>
+      <c r="EW55">
+        <v>0</v>
+      </c>
+      <c r="EX55">
+        <v>0</v>
+      </c>
+      <c r="EY55">
         <v>-2</v>
-      </c>
-      <c r="EP55">
-        <v>-2</v>
-      </c>
-      <c r="EQ55">
-        <v>-2</v>
-      </c>
-      <c r="ER55">
-        <v>-2</v>
-      </c>
-      <c r="ES55">
-        <v>-2</v>
-      </c>
-      <c r="ET55">
-        <v>-2</v>
-      </c>
-      <c r="EU55">
-        <v>-2</v>
-      </c>
-      <c r="EV55">
-        <v>-2</v>
-      </c>
-      <c r="EW55">
-        <v>-2</v>
-      </c>
-      <c r="EX55">
-        <v>-2</v>
-      </c>
-      <c r="EY55">
-        <v>-1</v>
       </c>
       <c r="EZ55">
         <v>0</v>
@@ -45529,97 +45670,97 @@
         <v>-1</v>
       </c>
       <c r="DJ59">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="DK59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DL59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DM59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DN59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DO59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DP59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DQ59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DR59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DS59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DT59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DU59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DV59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DW59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DX59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DY59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DZ59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EA59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EB59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EC59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="ED59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EE59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EF59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EG59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EH59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EI59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EJ59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EK59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EL59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EM59">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EN59">
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="EO59">
         <v>0</v>
@@ -79299,30 +79440,30 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A104:XFD1048576 A74:Y74 AX74:DL74 A1:XFD73 A75:DL103 DM74:XFD103">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+  <conditionalFormatting sqref="A104:XFD1048576 A74:Y74 AX74:DL74 A75:DL103 DM74:XFD103 A1:XFD73">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z74:AW74">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:IR103">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>-4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>